<commit_message>
Print using zebra language
</commit_message>
<xml_diff>
--- a/lib/data.xlsx
+++ b/lib/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>numero</t>
   </si>
@@ -31,72 +31,6 @@
   </si>
   <si>
     <t>711279</t>
-  </si>
-  <si>
-    <t>711280</t>
-  </si>
-  <si>
-    <t>711281</t>
-  </si>
-  <si>
-    <t>711282</t>
-  </si>
-  <si>
-    <t>711283</t>
-  </si>
-  <si>
-    <t>711284</t>
-  </si>
-  <si>
-    <t>711285</t>
-  </si>
-  <si>
-    <t>711286</t>
-  </si>
-  <si>
-    <t>711287</t>
-  </si>
-  <si>
-    <t>711288</t>
-  </si>
-  <si>
-    <t>711289</t>
-  </si>
-  <si>
-    <t>711290</t>
-  </si>
-  <si>
-    <t>711291</t>
-  </si>
-  <si>
-    <t>711292</t>
-  </si>
-  <si>
-    <t>711293</t>
-  </si>
-  <si>
-    <t>711294</t>
-  </si>
-  <si>
-    <t>711295</t>
-  </si>
-  <si>
-    <t>711296</t>
-  </si>
-  <si>
-    <t>711297</t>
-  </si>
-  <si>
-    <t>711298</t>
-  </si>
-  <si>
-    <t>711299</t>
-  </si>
-  <si>
-    <t>711300</t>
-  </si>
-  <si>
-    <t>711301</t>
   </si>
 </sst>
 </file>
@@ -385,180 +319,92 @@
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="2"/>

</xml_diff>